<commit_message>
add format for time-logs
</commit_message>
<xml_diff>
--- a/src/assets/reports/Attendance.xlsx
+++ b/src/assets/reports/Attendance.xlsx
@@ -4,65 +4,38 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>name</t>
+    <t>Code</t>
   </si>
   <si>
-    <t>code</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>First</t>
+    <t>Type</t>
   </si>
   <si>
-    <t>Check-out</t>
-  </si>
-  <si>
-    <t>Check-in</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>Third</t>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,18 +76,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,95 +373,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>